<commit_message>
💎style: Adjustment of default table styles.
</commit_message>
<xml_diff>
--- a/results/TEST_0_absolute_value_table.xlsx
+++ b/results/TEST_0_absolute_value_table.xlsx
@@ -66,8 +66,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00c3b6a1"/>
-        <bgColor rgb="00c3b6a1"/>
+        <fgColor rgb="00C5D9F1"/>
+        <bgColor rgb="00C5D9F1"/>
       </patternFill>
     </fill>
   </fills>
@@ -81,15 +81,15 @@
     </border>
     <border>
       <top style="medium">
-        <color rgb="0086754d"/>
+        <color rgb="00444444"/>
       </top>
       <bottom style="medium">
-        <color rgb="0086754d"/>
+        <color rgb="00444444"/>
       </bottom>
     </border>
     <border>
       <top style="medium">
-        <color rgb="0086754d"/>
+        <color rgb="00444444"/>
       </top>
     </border>
   </borders>

</xml_diff>